<commit_message>
Fixed RSquared for parameter estimates abundance model plotting
</commit_message>
<xml_diff>
--- a/Panels/parameter_estimates_Beta_Abundance.xlsx
+++ b/Panels/parameter_estimates_Beta_Abundance.xlsx
@@ -413,28 +413,28 @@
         </is>
       </c>
       <c r="B2">
-        <v>-5.825838863324705</v>
+        <v>-6.2659309253239</v>
       </c>
       <c r="C2">
-        <v>-0.6971591548838261</v>
+        <v>-0.5988942842363025</v>
       </c>
       <c r="D2">
-        <v>-0.01478506263232686</v>
+        <v>-0.0140986211690393</v>
       </c>
       <c r="E2">
-        <v>-0.4231702688990955</v>
+        <v>-0.395317187318695</v>
       </c>
       <c r="F2">
-        <v>0.007311242092792766</v>
+        <v>0.007248249644022577</v>
       </c>
       <c r="G2">
-        <v>0.1857629144000706</v>
+        <v>0.1951207373002259</v>
       </c>
       <c r="H2">
-        <v>0.009557910538579214</v>
+        <v>0.01087754231121822</v>
       </c>
       <c r="I2">
-        <v>-0.1006742654582948</v>
+        <v>-0.07928421786462415</v>
       </c>
     </row>
     <row r="3">
@@ -444,28 +444,28 @@
         </is>
       </c>
       <c r="B3">
-        <v>-10.94365151074486</v>
+        <v>-10.72164466035066</v>
       </c>
       <c r="C3">
-        <v>-0.6444982989925838</v>
+        <v>-0.8043154816306575</v>
       </c>
       <c r="D3">
-        <v>0.04193340185699471</v>
+        <v>0.04124935672767511</v>
       </c>
       <c r="E3">
-        <v>-0.8910485878605227</v>
+        <v>-0.8350964202807636</v>
       </c>
       <c r="F3">
-        <v>-0.03428214455678385</v>
+        <v>-0.03432429192355456</v>
       </c>
       <c r="G3">
-        <v>0.2771826912439125</v>
+        <v>0.2648233406737049</v>
       </c>
       <c r="H3">
-        <v>0.03839395962971425</v>
+        <v>0.03979806246669471</v>
       </c>
       <c r="I3">
-        <v>-0.2383505495108586</v>
+        <v>-0.2832089387179023</v>
       </c>
     </row>
     <row r="4">
@@ -475,28 +475,28 @@
         </is>
       </c>
       <c r="B4">
-        <v>1.700896959363607</v>
+        <v>2.043122287843016</v>
       </c>
       <c r="C4">
-        <v>-0.1155551448185213</v>
+        <v>-0.1112767069613757</v>
       </c>
       <c r="D4">
-        <v>-0.05871857844190417</v>
+        <v>-0.05932203237308012</v>
       </c>
       <c r="E4">
-        <v>-0.218928242112761</v>
+        <v>0.06625336085183849</v>
       </c>
       <c r="F4">
-        <v>-0.06949408924227654</v>
+        <v>-0.07003508609985085</v>
       </c>
       <c r="G4">
-        <v>-0.3347312498061811</v>
+        <v>-0.338410543024619</v>
       </c>
       <c r="H4">
-        <v>-0.06058039980386455</v>
+        <v>-0.06037784303232136</v>
       </c>
       <c r="I4">
-        <v>1.67684477430401</v>
+        <v>1.65365699251615</v>
       </c>
     </row>
     <row r="5">
@@ -506,28 +506,28 @@
         </is>
       </c>
       <c r="B5">
-        <v>-9.493959768132187</v>
+        <v>-9.508006568357688</v>
       </c>
       <c r="C5">
-        <v>-0.2381106005617386</v>
+        <v>-0.1681438044433469</v>
       </c>
       <c r="D5">
-        <v>-0.01631696761983516</v>
+        <v>-0.01522853408290514</v>
       </c>
       <c r="E5">
-        <v>-0.6276751162207481</v>
+        <v>-0.6748524692989257</v>
       </c>
       <c r="F5">
-        <v>-0.07404479068600647</v>
+        <v>-0.07290528571770309</v>
       </c>
       <c r="G5">
-        <v>0.04141277595138613</v>
+        <v>0.04581744617959855</v>
       </c>
       <c r="H5">
-        <v>0.0562559352289498</v>
+        <v>0.05543605725446554</v>
       </c>
       <c r="I5">
-        <v>0.1026580366741692</v>
+        <v>0.1340567878675038</v>
       </c>
     </row>
     <row r="6">
@@ -537,28 +537,28 @@
         </is>
       </c>
       <c r="B6">
-        <v>-10.1778035154372</v>
+        <v>-10.27501837697094</v>
       </c>
       <c r="C6">
-        <v>0.5454562657982888</v>
+        <v>0.4121991287101447</v>
       </c>
       <c r="D6">
-        <v>-0.01352298896726897</v>
+        <v>-0.01259309166135484</v>
       </c>
       <c r="E6">
-        <v>0.1029511158066901</v>
+        <v>-0.01814947604667764</v>
       </c>
       <c r="F6">
-        <v>0.02600389749195921</v>
+        <v>0.0259453283256228</v>
       </c>
       <c r="G6">
-        <v>0.2031327083697974</v>
+        <v>0.2227597874779113</v>
       </c>
       <c r="H6">
-        <v>0.02090963391085943</v>
+        <v>0.02026743534997227</v>
       </c>
       <c r="I6">
-        <v>0.3061569307617224</v>
+        <v>0.2977731179121011</v>
       </c>
     </row>
     <row r="7">
@@ -568,28 +568,28 @@
         </is>
       </c>
       <c r="B7">
-        <v>-6.651771351594745</v>
+        <v>-6.398771443458977</v>
       </c>
       <c r="C7">
-        <v>1.182614494949149</v>
+        <v>1.195711469806844</v>
       </c>
       <c r="D7">
-        <v>-0.000763605265615048</v>
+        <v>-0.0004365683546076519</v>
       </c>
       <c r="E7">
-        <v>0.1770566948544431</v>
+        <v>0.1833756311464365</v>
       </c>
       <c r="F7">
-        <v>0.006967124494470272</v>
+        <v>0.007098102094892961</v>
       </c>
       <c r="G7">
-        <v>0.08009971078092895</v>
+        <v>0.07520610624885114</v>
       </c>
       <c r="H7">
-        <v>0.02027008614188588</v>
+        <v>0.01843277933350791</v>
       </c>
       <c r="I7">
-        <v>0.1071225200687039</v>
+        <v>0.110225409380142</v>
       </c>
     </row>
     <row r="8">
@@ -599,28 +599,28 @@
         </is>
       </c>
       <c r="B8">
-        <v>-8.244674469146847</v>
+        <v>-8.414319109939104</v>
       </c>
       <c r="C8">
-        <v>1.772046764396567</v>
+        <v>1.713710700555608</v>
       </c>
       <c r="D8">
-        <v>-0.001231584751299507</v>
+        <v>-0.001685712123157412</v>
       </c>
       <c r="E8">
-        <v>0.4134269420952006</v>
+        <v>0.3518928857056302</v>
       </c>
       <c r="F8">
-        <v>0.004974764527813136</v>
+        <v>0.005271989081050034</v>
       </c>
       <c r="G8">
-        <v>0.05366752052419242</v>
+        <v>0.06802620777648208</v>
       </c>
       <c r="H8">
-        <v>0.02761135729406535</v>
+        <v>0.02866923596795208</v>
       </c>
       <c r="I8">
-        <v>0.3658761495729702</v>
+        <v>0.324948894735677</v>
       </c>
     </row>
     <row r="9">
@@ -630,28 +630,28 @@
         </is>
       </c>
       <c r="B9">
-        <v>-5.647158771822716</v>
+        <v>-5.003515765543416</v>
       </c>
       <c r="C9">
-        <v>2.029588126533735</v>
+        <v>2.094526694466488</v>
       </c>
       <c r="D9">
-        <v>-0.01226928188809841</v>
+        <v>-0.01313730066515563</v>
       </c>
       <c r="E9">
-        <v>0.6211644677289987</v>
+        <v>0.685502183251541</v>
       </c>
       <c r="F9">
-        <v>0.003167347822277109</v>
+        <v>0.003223352991792302</v>
       </c>
       <c r="G9">
-        <v>0.09623173029780528</v>
+        <v>0.07947413272493827</v>
       </c>
       <c r="H9">
-        <v>0.01170348954034164</v>
+        <v>0.00889948454518103</v>
       </c>
       <c r="I9">
-        <v>0.1243344654865459</v>
+        <v>0.1126379670019341</v>
       </c>
     </row>
     <row r="10">
@@ -661,28 +661,28 @@
         </is>
       </c>
       <c r="B10">
-        <v>-5.994531176823412</v>
+        <v>-5.269847661638758</v>
       </c>
       <c r="C10">
-        <v>0.9492854417775023</v>
+        <v>0.9520113185559916</v>
       </c>
       <c r="D10">
-        <v>0.0008917253992286373</v>
+        <v>3.830684377228642e-05</v>
       </c>
       <c r="E10">
-        <v>0.1645139469633357</v>
+        <v>0.2634160282476582</v>
       </c>
       <c r="F10">
-        <v>0.00564386231358575</v>
+        <v>0.005670951710796803</v>
       </c>
       <c r="G10">
-        <v>-0.02612719532771465</v>
+        <v>-0.04569753286671877</v>
       </c>
       <c r="H10">
-        <v>0.01365820067958766</v>
+        <v>0.01000221892351058</v>
       </c>
       <c r="I10">
-        <v>0.1207800950192279</v>
+        <v>0.1419500704792796</v>
       </c>
     </row>
     <row r="11">
@@ -692,28 +692,28 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.9916313425565998</v>
+        <v>-0.08081600901010699</v>
       </c>
       <c r="C11">
-        <v>-0.01735553288652507</v>
+        <v>0.1589588998973643</v>
       </c>
       <c r="D11">
-        <v>-0.01439334671414819</v>
+        <v>-0.01393218973184394</v>
       </c>
       <c r="E11">
-        <v>0.1621367133256543</v>
+        <v>0.3801712135025674</v>
       </c>
       <c r="F11">
-        <v>-0.003909944659101316</v>
+        <v>-0.001320550156367274</v>
       </c>
       <c r="G11">
-        <v>0.105335363946113</v>
+        <v>0.08587700128372658</v>
       </c>
       <c r="H11">
-        <v>-0.00681024362982461</v>
+        <v>-0.01073643459022128</v>
       </c>
       <c r="I11">
-        <v>-0.510043539232475</v>
+        <v>-0.5385430273393251</v>
       </c>
     </row>
     <row r="12">
@@ -723,28 +723,28 @@
         </is>
       </c>
       <c r="B12">
-        <v>-4.760252134784721</v>
+        <v>-3.737562131959649</v>
       </c>
       <c r="C12">
-        <v>1.119486880775421</v>
+        <v>1.198938645820635</v>
       </c>
       <c r="D12">
-        <v>-0.00635508550199436</v>
+        <v>-0.005669955498870197</v>
       </c>
       <c r="E12">
-        <v>0.3633552267238573</v>
+        <v>0.4994194862424781</v>
       </c>
       <c r="F12">
-        <v>-0.001565602943012976</v>
+        <v>-0.002439953630670999</v>
       </c>
       <c r="G12">
-        <v>-0.002647745951756673</v>
+        <v>-0.02565983010042778</v>
       </c>
       <c r="H12">
-        <v>0.004730172998240742</v>
+        <v>-0.000219298539083331</v>
       </c>
       <c r="I12">
-        <v>0.05067519869145914</v>
+        <v>0.0526718488413991</v>
       </c>
     </row>
     <row r="13">
@@ -754,28 +754,28 @@
         </is>
       </c>
       <c r="B13">
-        <v>-7.157215705437404</v>
+        <v>-6.818080241163051</v>
       </c>
       <c r="C13">
-        <v>-1.373470201318132</v>
+        <v>-1.542599298827969</v>
       </c>
       <c r="D13">
-        <v>0.01788185270649164</v>
+        <v>0.01911266511003648</v>
       </c>
       <c r="E13">
-        <v>-0.310625956251363</v>
+        <v>-0.2324557779673498</v>
       </c>
       <c r="F13">
-        <v>0.02714658981082592</v>
+        <v>0.024870453764421</v>
       </c>
       <c r="G13">
-        <v>0.05563370030775162</v>
+        <v>0.0434807513647179</v>
       </c>
       <c r="H13">
-        <v>-0.01262959605220165</v>
+        <v>-0.009920020765254346</v>
       </c>
       <c r="I13">
-        <v>0.5213435865583225</v>
+        <v>0.485676954731076</v>
       </c>
     </row>
   </sheetData>
@@ -845,28 +845,28 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.05159375</v>
+        <v>0.04284375</v>
       </c>
       <c r="C2">
-        <v>0.05996875</v>
+        <v>0.08712499999999999</v>
       </c>
       <c r="D2">
-        <v>0.0040625</v>
+        <v>0.0043125</v>
       </c>
       <c r="E2">
-        <v>0.050375</v>
+        <v>0.05775</v>
       </c>
       <c r="F2">
-        <v>0.91909375</v>
+        <v>0.919875</v>
       </c>
       <c r="G2">
-        <v>0.97246875</v>
+        <v>0.9770624999999999</v>
       </c>
       <c r="H2">
-        <v>0.756625</v>
+        <v>0.7776875</v>
       </c>
       <c r="I2">
-        <v>0.241125</v>
+        <v>0.28696875</v>
       </c>
     </row>
     <row r="3">
@@ -876,28 +876,28 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.00584375</v>
+        <v>0.008718750000000001</v>
       </c>
       <c r="C3">
-        <v>0.01725</v>
+        <v>0.0068125</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.02134375</v>
+        <v>0.07178125</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.000125</v>
       </c>
       <c r="G3">
-        <v>0.9880625</v>
+        <v>0.9799687500000001</v>
       </c>
       <c r="H3">
-        <v>0.9948125</v>
+        <v>0.99290625</v>
       </c>
       <c r="I3">
-        <v>0.0199375</v>
+        <v>0.009124999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -907,16 +907,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.661625</v>
+        <v>0.69171875</v>
       </c>
       <c r="C4">
-        <v>0.3586875</v>
+        <v>0.36009375</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.4199375</v>
+        <v>0.52209375</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -938,28 +938,28 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.0001875</v>
+        <v>9.375e-05</v>
       </c>
       <c r="C5">
-        <v>0.137875</v>
+        <v>0.24621875</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.20821875</v>
+        <v>0.19190625</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.77225</v>
+        <v>0.79925</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0.834125</v>
+        <v>0.87790625</v>
       </c>
     </row>
     <row r="6">
@@ -969,28 +969,28 @@
         </is>
       </c>
       <c r="B6">
-        <v>6.25e-05</v>
+        <v>9.375e-05</v>
       </c>
       <c r="C6">
-        <v>0.894375</v>
+        <v>0.84403125</v>
       </c>
       <c r="D6">
-        <v>0.00053125</v>
+        <v>0.00128125</v>
       </c>
       <c r="E6">
-        <v>0.6345</v>
+        <v>0.4939375</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.99496875</v>
+        <v>0.9975000000000001</v>
       </c>
       <c r="H6">
-        <v>0.9755625</v>
+        <v>0.9672500000000001</v>
       </c>
       <c r="I6">
-        <v>0.999</v>
+        <v>0.99865625</v>
       </c>
     </row>
     <row r="7">
@@ -1000,28 +1000,28 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.04121875</v>
+        <v>0.051</v>
       </c>
       <c r="C7">
-        <v>0.99496875</v>
+        <v>0.996625</v>
       </c>
       <c r="D7">
-        <v>0.427625</v>
+        <v>0.457375</v>
       </c>
       <c r="E7">
-        <v>0.79396875</v>
+        <v>0.78303125</v>
       </c>
       <c r="F7">
-        <v>0.96421875</v>
+        <v>0.9649375</v>
       </c>
       <c r="G7">
-        <v>0.79384375</v>
+        <v>0.7708125</v>
       </c>
       <c r="H7">
-        <v>0.9325625</v>
+        <v>0.90790625</v>
       </c>
       <c r="I7">
-        <v>0.7866562499999999</v>
+        <v>0.80221875</v>
       </c>
     </row>
     <row r="8">
@@ -1031,28 +1031,28 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.0174375</v>
+        <v>0.01546875</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.3446875</v>
+        <v>0.304625</v>
       </c>
       <c r="E8">
-        <v>0.9771875</v>
+        <v>0.94271875</v>
       </c>
       <c r="F8">
-        <v>0.9519375</v>
+        <v>0.9545625</v>
       </c>
       <c r="G8">
-        <v>0.70078125</v>
+        <v>0.7409375</v>
       </c>
       <c r="H8">
-        <v>0.9791875</v>
+        <v>0.97975</v>
       </c>
       <c r="I8">
-        <v>0.99990625</v>
+        <v>0.999375</v>
       </c>
     </row>
     <row r="9">
@@ -1062,28 +1062,28 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.07609375</v>
+        <v>0.1104375</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>9.375e-05</v>
+        <v>0.000125</v>
       </c>
       <c r="E9">
-        <v>0.98759375</v>
+        <v>0.985375</v>
       </c>
       <c r="F9">
-        <v>0.826875</v>
+        <v>0.81459375</v>
       </c>
       <c r="G9">
-        <v>0.81346875</v>
+        <v>0.7610625</v>
       </c>
       <c r="H9">
-        <v>0.80540625</v>
+        <v>0.735625</v>
       </c>
       <c r="I9">
-        <v>0.83365625</v>
+        <v>0.79571875</v>
       </c>
     </row>
     <row r="10">
@@ -1093,28 +1093,28 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.1041875</v>
+        <v>0.140375</v>
       </c>
       <c r="C10">
-        <v>0.90096875</v>
+        <v>0.90821875</v>
       </c>
       <c r="D10">
-        <v>0.548</v>
+        <v>0.502</v>
       </c>
       <c r="E10">
-        <v>0.6579375</v>
+        <v>0.75125</v>
       </c>
       <c r="F10">
-        <v>0.7860625</v>
+        <v>0.7905624999999999</v>
       </c>
       <c r="G10">
-        <v>0.4395</v>
+        <v>0.384125</v>
       </c>
       <c r="H10">
-        <v>0.788</v>
+        <v>0.7185</v>
       </c>
       <c r="I10">
-        <v>0.7221562500000001</v>
+        <v>0.737125</v>
       </c>
     </row>
     <row r="11">
@@ -1124,28 +1124,28 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.41696875</v>
+        <v>0.473</v>
       </c>
       <c r="C11">
-        <v>0.5014999999999999</v>
+        <v>0.57984375</v>
       </c>
       <c r="D11">
-        <v>0.1084375</v>
+        <v>0.10484375</v>
       </c>
       <c r="E11">
-        <v>0.6210625</v>
+        <v>0.7761875</v>
       </c>
       <c r="F11">
-        <v>0.3785</v>
+        <v>0.46271875</v>
       </c>
       <c r="G11">
-        <v>0.73625</v>
+        <v>0.6921875</v>
       </c>
       <c r="H11">
-        <v>0.39946875</v>
+        <v>0.3445</v>
       </c>
       <c r="I11">
-        <v>0.01828125</v>
+        <v>0.01484375</v>
       </c>
     </row>
     <row r="12">
@@ -1155,28 +1155,28 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.17096875</v>
+        <v>0.2384375</v>
       </c>
       <c r="C12">
-        <v>0.92665625</v>
+        <v>0.9348125</v>
       </c>
       <c r="D12">
-        <v>0.27115625</v>
+        <v>0.3039375</v>
       </c>
       <c r="E12">
-        <v>0.78440625</v>
+        <v>0.839</v>
       </c>
       <c r="F12">
-        <v>0.457375</v>
+        <v>0.42525</v>
       </c>
       <c r="G12">
-        <v>0.50434375</v>
+        <v>0.4446875</v>
       </c>
       <c r="H12">
-        <v>0.596375</v>
+        <v>0.50109375</v>
       </c>
       <c r="I12">
-        <v>0.57196875</v>
+        <v>0.5748124999999999</v>
       </c>
     </row>
     <row r="13">
@@ -1186,28 +1186,28 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.099</v>
+        <v>0.11515625</v>
       </c>
       <c r="C13">
-        <v>0.0383125</v>
+        <v>0.03646875</v>
       </c>
       <c r="D13">
-        <v>0.99553125</v>
+        <v>0.9975937499999999</v>
       </c>
       <c r="E13">
-        <v>0.22725</v>
+        <v>0.31625</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0.647125</v>
+        <v>0.615125</v>
       </c>
       <c r="H13">
-        <v>0.27771875</v>
+        <v>0.319625</v>
       </c>
       <c r="I13">
-        <v>0.99834375</v>
+        <v>0.99684375</v>
       </c>
     </row>
   </sheetData>
@@ -1277,28 +1277,28 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.94840625</v>
+        <v>0.95715625</v>
       </c>
       <c r="C2">
-        <v>0.94003125</v>
+        <v>0.912875</v>
       </c>
       <c r="D2">
-        <v>0.9959375</v>
+        <v>0.9956874999999999</v>
       </c>
       <c r="E2">
-        <v>0.9496250000000001</v>
+        <v>0.94225</v>
       </c>
       <c r="F2">
-        <v>0.08090625</v>
+        <v>0.080125</v>
       </c>
       <c r="G2">
-        <v>0.02753125</v>
+        <v>0.0229375</v>
       </c>
       <c r="H2">
-        <v>0.243375</v>
+        <v>0.2223125</v>
       </c>
       <c r="I2">
-        <v>0.758875</v>
+        <v>0.71303125</v>
       </c>
     </row>
     <row r="3">
@@ -1308,28 +1308,28 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.99415625</v>
+        <v>0.99128125</v>
       </c>
       <c r="C3">
-        <v>0.98275</v>
+        <v>0.9931875</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.97865625</v>
+        <v>0.92821875</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.999875</v>
       </c>
       <c r="G3">
-        <v>0.0119375</v>
+        <v>0.02003125</v>
       </c>
       <c r="H3">
-        <v>0.0051875</v>
+        <v>0.00709375</v>
       </c>
       <c r="I3">
-        <v>0.9800624999999999</v>
+        <v>0.990875</v>
       </c>
     </row>
     <row r="4">
@@ -1339,16 +1339,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.338375</v>
+        <v>0.30828125</v>
       </c>
       <c r="C4">
-        <v>0.6413125</v>
+        <v>0.63990625</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.5800625</v>
+        <v>0.47790625</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1370,28 +1370,28 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.9998125</v>
+        <v>0.99990625</v>
       </c>
       <c r="C5">
-        <v>0.862125</v>
+        <v>0.75378125</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.79178125</v>
+        <v>0.8080937500000001</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.22775</v>
+        <v>0.20075</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.165875</v>
+        <v>0.12209375</v>
       </c>
     </row>
     <row r="6">
@@ -1401,28 +1401,28 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.9999375</v>
+        <v>0.99990625</v>
       </c>
       <c r="C6">
-        <v>0.105625</v>
+        <v>0.15596875</v>
       </c>
       <c r="D6">
-        <v>0.99946875</v>
+        <v>0.99871875</v>
       </c>
       <c r="E6">
-        <v>0.3655</v>
+        <v>0.5060625</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.00503125</v>
+        <v>0.0025</v>
       </c>
       <c r="H6">
-        <v>0.0244375</v>
+        <v>0.03275</v>
       </c>
       <c r="I6">
-        <v>0.001</v>
+        <v>0.00134375</v>
       </c>
     </row>
     <row r="7">
@@ -1432,28 +1432,28 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.95878125</v>
+        <v>0.949</v>
       </c>
       <c r="C7">
-        <v>0.00503125</v>
+        <v>0.003375</v>
       </c>
       <c r="D7">
-        <v>0.572375</v>
+        <v>0.542625</v>
       </c>
       <c r="E7">
-        <v>0.20603125</v>
+        <v>0.21696875</v>
       </c>
       <c r="F7">
-        <v>0.03578125</v>
+        <v>0.0350625</v>
       </c>
       <c r="G7">
-        <v>0.20615625</v>
+        <v>0.2291875</v>
       </c>
       <c r="H7">
-        <v>0.0674375</v>
+        <v>0.09209375</v>
       </c>
       <c r="I7">
-        <v>0.21334375</v>
+        <v>0.19778125</v>
       </c>
     </row>
     <row r="8">
@@ -1463,28 +1463,28 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.9825625</v>
+        <v>0.98453125</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.6553125</v>
+        <v>0.695375</v>
       </c>
       <c r="E8">
-        <v>0.0228125</v>
+        <v>0.05728125</v>
       </c>
       <c r="F8">
-        <v>0.0480625</v>
+        <v>0.0454375</v>
       </c>
       <c r="G8">
-        <v>0.29921875</v>
+        <v>0.2590625</v>
       </c>
       <c r="H8">
-        <v>0.0208125</v>
+        <v>0.02025</v>
       </c>
       <c r="I8">
-        <v>9.375e-05</v>
+        <v>0.000625</v>
       </c>
     </row>
     <row r="9">
@@ -1494,28 +1494,28 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.92390625</v>
+        <v>0.8895625</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.99990625</v>
+        <v>0.999875</v>
       </c>
       <c r="E9">
-        <v>0.01240625</v>
+        <v>0.014625</v>
       </c>
       <c r="F9">
-        <v>0.173125</v>
+        <v>0.18540625</v>
       </c>
       <c r="G9">
-        <v>0.18653125</v>
+        <v>0.2389375</v>
       </c>
       <c r="H9">
-        <v>0.19459375</v>
+        <v>0.264375</v>
       </c>
       <c r="I9">
-        <v>0.16634375</v>
+        <v>0.20428125</v>
       </c>
     </row>
     <row r="10">
@@ -1525,28 +1525,28 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.8958125</v>
+        <v>0.859625</v>
       </c>
       <c r="C10">
-        <v>0.09903125</v>
+        <v>0.09178124999999999</v>
       </c>
       <c r="D10">
-        <v>0.452</v>
+        <v>0.498</v>
       </c>
       <c r="E10">
-        <v>0.3420625</v>
+        <v>0.24875</v>
       </c>
       <c r="F10">
-        <v>0.2139375</v>
+        <v>0.2094375</v>
       </c>
       <c r="G10">
-        <v>0.5605</v>
+        <v>0.615875</v>
       </c>
       <c r="H10">
-        <v>0.212</v>
+        <v>0.2815</v>
       </c>
       <c r="I10">
-        <v>0.27784375</v>
+        <v>0.262875</v>
       </c>
     </row>
     <row r="11">
@@ -1556,28 +1556,28 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.58303125</v>
+        <v>0.527</v>
       </c>
       <c r="C11">
-        <v>0.4985</v>
+        <v>0.42015625</v>
       </c>
       <c r="D11">
-        <v>0.8915625</v>
+        <v>0.89515625</v>
       </c>
       <c r="E11">
-        <v>0.3789375</v>
+        <v>0.2238125</v>
       </c>
       <c r="F11">
-        <v>0.6215000000000001</v>
+        <v>0.53728125</v>
       </c>
       <c r="G11">
-        <v>0.26375</v>
+        <v>0.3078125</v>
       </c>
       <c r="H11">
-        <v>0.60053125</v>
+        <v>0.6555</v>
       </c>
       <c r="I11">
-        <v>0.98171875</v>
+        <v>0.98515625</v>
       </c>
     </row>
     <row r="12">
@@ -1587,28 +1587,28 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.82903125</v>
+        <v>0.7615625</v>
       </c>
       <c r="C12">
-        <v>0.07334375</v>
+        <v>0.0651875</v>
       </c>
       <c r="D12">
-        <v>0.72884375</v>
+        <v>0.6960625</v>
       </c>
       <c r="E12">
-        <v>0.21559375</v>
+        <v>0.161</v>
       </c>
       <c r="F12">
-        <v>0.542625</v>
+        <v>0.57475</v>
       </c>
       <c r="G12">
-        <v>0.49565625</v>
+        <v>0.5553125</v>
       </c>
       <c r="H12">
-        <v>0.403625</v>
+        <v>0.49890625</v>
       </c>
       <c r="I12">
-        <v>0.42803125</v>
+        <v>0.4251875</v>
       </c>
     </row>
     <row r="13">
@@ -1618,28 +1618,28 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.901</v>
+        <v>0.88484375</v>
       </c>
       <c r="C13">
-        <v>0.9616875</v>
+        <v>0.96353125</v>
       </c>
       <c r="D13">
-        <v>0.00446875</v>
+        <v>0.00240625</v>
       </c>
       <c r="E13">
-        <v>0.77275</v>
+        <v>0.68375</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.352875</v>
+        <v>0.384875</v>
       </c>
       <c r="H13">
-        <v>0.72228125</v>
+        <v>0.680375</v>
       </c>
       <c r="I13">
-        <v>0.00165625</v>
+        <v>0.00315625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>